<commit_message>
Se agregan costos de vuelos y comida
</commit_message>
<xml_diff>
--- a/Ventas/Propuesta Económica/Prupuesta Económica V5.xlsx
+++ b/Ventas/Propuesta Económica/Prupuesta Económica V5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AntirShadow\Documents\GitHub\ProyectoRedes\Ventas\Propuesta Económica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA2F9B9-CDC6-4155-95B9-17E1E2D81B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4A290E-627C-4DF1-A81E-A50915562009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>PROPUESTA ECONÓMICA</t>
   </si>
@@ -86,29 +86,39 @@
     <t>https://articulo.mercadolibre.com.mx/MLM-1300594446-100-piezas-cable-cat6-rj45-conectores-cat6-cat5e-rj45utp-_JM#position=5&amp;search_layout=grid&amp;type=item&amp;tracking_id=d26aa09f-a4f7-44a7-b455-ec3998c093b6</t>
   </si>
   <si>
-    <t>Viaje Guadalaja VivaAerobus</t>
-  </si>
-  <si>
-    <t>Viaje Veracruz</t>
-  </si>
-  <si>
-    <t>Viaje Monterrey</t>
-  </si>
-  <si>
-    <t>Viaje Querétaro</t>
-  </si>
-  <si>
     <t>Viáticos diarios P/Persona</t>
+  </si>
+  <si>
+    <t>DESCUENTOS</t>
+  </si>
+  <si>
+    <t>https://paquetes.cityexpress.com/reservar/detalle-reservacion-paquetes</t>
+  </si>
+  <si>
+    <t>Veracruz Vuelo y Hospedaje Con Desayuno 2 Personas</t>
+  </si>
+  <si>
+    <t>Guadalajara Vuelo y Hospedaje Con Desayuno 2 Personas</t>
+  </si>
+  <si>
+    <t>Querétaro Vuelo y Hospedaje Con Desayuno 2 Personas</t>
+  </si>
+  <si>
+    <t>Monterrey Vuelo y Hospedaje Con Desayuno 2 Personas</t>
+  </si>
+  <si>
+    <t>Camioneta transporte objetos y movilidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -190,6 +200,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -270,14 +287,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -289,16 +307,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -313,24 +325,74 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Bueno" xfId="3" builtinId="26"/>
     <cellStyle name="Celda de comprobación" xfId="4" builtinId="23"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="5" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -449,15 +511,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{260CAE73-387D-4728-94B4-6CA7A8B0F168}" name="Tabla1" displayName="Tabla1" ref="A2:F14" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A2:F14" xr:uid="{260CAE73-387D-4728-94B4-6CA7A8B0F168}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F6F1872D-62D6-465A-9EB6-D1E64C7FD1EA}" name="N ITEM" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{05A4D583-BEEA-420F-8DC9-DB385506B921}" name="DESCRIPCIÓN" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{16119888-3FB2-48ED-BB90-CB4798528804}" name="NO. DE PARTE" dataDxfId="3" dataCellStyle="Moneda"/>
-    <tableColumn id="4" xr3:uid="{17DCB875-5E51-4C91-B16E-78560646B0A5}" name="PRECIO UNITARIO" dataDxfId="2" dataCellStyle="Moneda"/>
-    <tableColumn id="5" xr3:uid="{DAECB143-E7A2-4C29-91CB-3EBCE0FFA4CA}" name="SUBTOTAL" dataDxfId="1" dataCellStyle="Moneda"/>
-    <tableColumn id="6" xr3:uid="{CDC3B595-CE04-4E68-9C64-2BFC0D49CE76}" name="LINK" dataDxfId="0" dataCellStyle="Hipervínculo"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{260CAE73-387D-4728-94B4-6CA7A8B0F168}" name="Tabla1" displayName="Tabla1" ref="A2:H14" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A2:H14" xr:uid="{260CAE73-387D-4728-94B4-6CA7A8B0F168}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{F6F1872D-62D6-465A-9EB6-D1E64C7FD1EA}" name="N ITEM" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{05A4D583-BEEA-420F-8DC9-DB385506B921}" name="DESCRIPCIÓN" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{16119888-3FB2-48ED-BB90-CB4798528804}" name="NO. DE PARTE" dataDxfId="4" dataCellStyle="Moneda"/>
+    <tableColumn id="4" xr3:uid="{17DCB875-5E51-4C91-B16E-78560646B0A5}" name="PRECIO UNITARIO" dataDxfId="3" dataCellStyle="Moneda"/>
+    <tableColumn id="8" xr3:uid="{9504F072-2CE8-4154-ADE6-5071E962149C}" name="DESCUENTOS"/>
+    <tableColumn id="5" xr3:uid="{DAECB143-E7A2-4C29-91CB-3EBCE0FFA4CA}" name="SUBTOTAL" dataDxfId="2" dataCellStyle="Moneda"/>
+    <tableColumn id="10" xr3:uid="{B913AF07-4667-4467-8BAC-58B0321E83ED}" name="TOTAL" dataDxfId="0" dataCellStyle="Moneda">
+      <calculatedColumnFormula>(C3*D3)*(100/100)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{CDC3B595-CE04-4E68-9C64-2BFC0D49CE76}" name="LINK" dataDxfId="1" dataCellStyle="Hipervínculo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -664,33 +730,37 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="46.2" x14ac:dyDescent="0.85">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:8" ht="46.2" x14ac:dyDescent="0.85">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -703,258 +773,385 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>15</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="16">
         <v>8969</v>
       </c>
-      <c r="E3" s="8">
-        <f t="shared" ref="E3:E8" si="0">C3*D3</f>
+      <c r="E3" s="20">
+        <v>15</v>
+      </c>
+      <c r="F3" s="14">
+        <f>C3*D3</f>
         <v>134535</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="18">
+        <f t="shared" ref="G3:G11" si="0">(C3*D3)*(100/100)</f>
+        <v>134535</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>5</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="16">
         <v>11310</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="20">
+        <v>5</v>
+      </c>
+      <c r="F4" s="14">
+        <f>C4*D4</f>
+        <v>56550</v>
+      </c>
+      <c r="G4" s="18">
         <f t="shared" si="0"/>
         <v>56550</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>3</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="14">
         <v>30000</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="14">
+        <f>C5*D5</f>
+        <v>90000</v>
+      </c>
+      <c r="G5" s="18">
         <f t="shared" si="0"/>
         <v>90000</v>
       </c>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>6</v>
-      </c>
-      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>9</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="14">
         <v>1149</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="20">
+        <v>10</v>
+      </c>
+      <c r="F6" s="14">
+        <f>C6*D6</f>
+        <v>10341</v>
+      </c>
+      <c r="G6" s="18">
         <f t="shared" si="0"/>
         <v>10341</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="7">
         <v>5</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="14">
         <v>152.28</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="20">
+        <v>0</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" ref="F7:F12" si="1">C7*D7</f>
+        <v>761.4</v>
+      </c>
+      <c r="G7" s="18">
         <f t="shared" si="0"/>
         <v>761.4</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="H7" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7">
+        <v>120</v>
+      </c>
+      <c r="D8" s="14">
+        <v>500</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="G8" s="18">
+        <f t="shared" si="0"/>
+        <v>60000</v>
+      </c>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7">
+        <v>15</v>
+      </c>
+      <c r="D9" s="14">
+        <v>2034.933</v>
+      </c>
+      <c r="E9" s="21">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="1"/>
+        <v>30523.994999999999</v>
+      </c>
+      <c r="G9" s="18">
+        <f t="shared" si="0"/>
+        <v>30523.994999999999</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="D8" s="8">
-        <f>1323+178.67+1125</f>
-        <v>2626.67</v>
-      </c>
-      <c r="E8" s="8">
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="17">
+        <v>15</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1939.4</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="1"/>
+        <v>29091</v>
+      </c>
+      <c r="G10" s="18">
         <f t="shared" si="0"/>
-        <v>5253.34</v>
-      </c>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+        <v>29091</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="B11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="17">
+        <v>15</v>
+      </c>
+      <c r="D11" s="15">
+        <v>1945.93</v>
+      </c>
+      <c r="E11" s="21">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="1"/>
+        <v>29188.95</v>
+      </c>
+      <c r="G11" s="18">
+        <f t="shared" si="0"/>
+        <v>29188.95</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="17">
+        <v>15</v>
+      </c>
+      <c r="D12" s="15">
+        <v>2141.3330000000001</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0</v>
+      </c>
+      <c r="F12" s="14">
+        <f t="shared" si="1"/>
+        <v>32119.995000000003</v>
+      </c>
+      <c r="G12" s="18">
+        <f t="shared" ref="G10:G12" si="2">(C12*D12)*(100/100)</f>
+        <v>32119.995000000003</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+    </row>
+    <row r="13" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="B13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="17">
+        <v>4</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="22">
+        <f t="shared" ref="G13:G14" si="3">(C13*D13)*(100/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="9">
-        <v>8</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>13</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>14</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="15">
-        <f>SUM(E3:E14)</f>
-        <v>297440.74000000005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:4" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:4" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F35" s="2"/>
+      <c r="B17" s="11">
+        <f>SUM(G3:G14)</f>
+        <v>473111.34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="21" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{2421FD61-C521-45B2-8DF5-B7B485BF9E38}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{D9DB3FEB-3A05-490A-A601-E4659876CB25}"/>
-    <hyperlink ref="F6" r:id="rId3" xr:uid="{D18119C8-5FA6-4F43-8CD8-2A77CC41275D}"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{2421FD61-C521-45B2-8DF5-B7B485BF9E38}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{D9DB3FEB-3A05-490A-A601-E4659876CB25}"/>
+    <hyperlink ref="H6" r:id="rId3" xr:uid="{D18119C8-5FA6-4F43-8CD8-2A77CC41275D}"/>
+    <hyperlink ref="H10" r:id="rId4" xr:uid="{9BE40A90-D202-4C44-8466-BCB4BDBFE904}"/>
+    <hyperlink ref="H12" r:id="rId5" xr:uid="{A7BF6B39-7EEC-4D0C-A1BF-9776AEF5C3D7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización Propuesta Económica V5
</commit_message>
<xml_diff>
--- a/Ventas/Propuesta Económica/Prupuesta Económica V5.xlsx
+++ b/Ventas/Propuesta Económica/Prupuesta Económica V5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AntirShadow\Documents\GitHub\ProyectoRedes\Ventas\Propuesta Económica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\AntirShadow\Documents\GitHub\ProyectoRedes\Ventas\Propuesta Económica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4A290E-627C-4DF1-A81E-A50915562009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA36B24-2EF2-4609-A043-47B40D1E5EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2340" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>PROPUESTA ECONÓMICA</t>
   </si>
@@ -107,7 +107,137 @@
     <t>Monterrey Vuelo y Hospedaje Con Desayuno 2 Personas</t>
   </si>
   <si>
-    <t>Camioneta transporte objetos y movilidad</t>
+    <t>https://www.priceline.com/rentalcars/Mexico%20City%20Mexico/Mexico%20City%20Mexico/20230516-10%3A00/20230530-10%3A00/list?detailsKey=MEXC001~MEXC001~R~N~~18822ce833f~~refCode-22-a769e839-1bbd-4f9f-b851-b7d56fef1fd1~20230516T10%3A00~20230530T10%3A00~AV~FQMR~USD~1068.52~~~~~878.00~1187.55~~*&amp;preferredPartnerCode=AV&amp;refid=PLKAYAK&amp;refclickid=CSR_RC%7CAvis%20Rent%20a%20Car%7C*Q**%7CMEXC001%7CMEXC001%7CPL%7C000%7C14%7Ctrue%7CRT%7CKC%3AsZFr71f8tJ8qTJz_MDLToA&amp;utm_medium=SHOP_PPC&amp;utm_source=PLKAYAK&amp;utm_term=CSR_RC%7CAvis%20Rent%20a%20Car%7C*Q**%7CMEXC001%7CMEXC001%7CPL%7C000%7C14%7Ctrue%7CRT%7CKC%3AsZFr71f8tJ8qTJz_MDLToA&amp;utm_content=CMP2&amp;utm_campaign=Car_Contract&amp;currencycode=USD&amp;carclass=FQMR&amp;dct=&amp;locale=&amp;pos=US&amp;currencyCode=USD&amp;slingshot=1774</t>
+  </si>
+  <si>
+    <t>Gasolina Monterrey ida y vuelta</t>
+  </si>
+  <si>
+    <t>Gasolina Guadalajara ida y vuelta</t>
+  </si>
+  <si>
+    <t>Gasolina Querétaro ida y vuelta</t>
+  </si>
+  <si>
+    <t>Gasolina Veracruz ida y vuelta</t>
+  </si>
+  <si>
+    <t>Gastos movilidad</t>
+  </si>
+  <si>
+    <t>https://www.distancial.com/Map/Ciudad%20de%20mexico/Queretaro</t>
+  </si>
+  <si>
+    <t>https://www.distancial.com/Map/Ciudad%20de%20mexico/Veracruz</t>
+  </si>
+  <si>
+    <t>https://www.distancial.com/Map/Ciudad%20de%20mexico/Jalisco</t>
+  </si>
+  <si>
+    <t>https://www.distancial.com/distancia-de-cdmx-a-monterrey</t>
+  </si>
+  <si>
+    <t>Pago chofer 15 días</t>
+  </si>
+  <si>
+    <t>Porcentaje de error</t>
+  </si>
+  <si>
+    <t>Camioneta transporte Accesorios y Movilidad</t>
+  </si>
+  <si>
+    <t>Porcentaje Ganancia</t>
+  </si>
+  <si>
+    <t>Venta</t>
+  </si>
+  <si>
+    <t>Ganacia</t>
+  </si>
+  <si>
+    <t>Ganancia Bruta Por Persona</t>
+  </si>
+  <si>
+    <t>Dolares</t>
+  </si>
+  <si>
+    <t>Tipo de cambio</t>
+  </si>
+  <si>
+    <t>Pesos</t>
+  </si>
+  <si>
+    <t>Suma</t>
+  </si>
+  <si>
+    <t>Vigencia</t>
+  </si>
+  <si>
+    <t>2 semanas</t>
+  </si>
+  <si>
+    <t>Dólares</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total USD</t>
+  </si>
+  <si>
+    <t>Pago inicial: 25%</t>
+  </si>
+  <si>
+    <t>Diseño de red: 30%</t>
+  </si>
+  <si>
+    <t>Mantenimiento Preventivo</t>
+  </si>
+  <si>
+    <t>Compra e instalación de equipos de red: 40%</t>
+  </si>
+  <si>
+    <t>Monitoreo 1: 2.5%</t>
+  </si>
+  <si>
+    <t>Monitoreo 2: 2.5%</t>
+  </si>
+  <si>
+    <t>Total Proyecto Peso y Dolar</t>
+  </si>
+  <si>
+    <t>Porcentajes</t>
+  </si>
+  <si>
+    <t>Ganancia por Persona</t>
+  </si>
+  <si>
+    <t>Ganancias del Proyecto</t>
+  </si>
+  <si>
+    <t>Pagos Desglozados</t>
+  </si>
+  <si>
+    <t>Descripción Planes de Pago</t>
+  </si>
+  <si>
+    <t>Pago inicial: 25% del costo total del proyecto ($33,189.54 USD) al momento de firmar el contrato.
+Diseño de red: 30% del costo total del proyecto ($39,827.443 USD) al completar el diseño de red y entregarlo al cliente para su aprobación.
+Compra e instalación de equipos de red: 40% del costo total del proyecto ($53,103.26 USD) al completar la compra e instalación de los equipos de red en los 5 diferentes centros de la república.
+Monitoreo preventivo: 2.5% del costo total del proyecto ($3,318.95 USD) al completar el primer monitoreo preventivo, medio año después de la instalación de los equipos de red.
+Pago final: 2.5% del costo total del proyecto ($3,318.95) al completar el segundo monitoreo preventivo, 1 año después de la instalación de los equipos de red.</t>
+  </si>
+  <si>
+    <t>Medios De Pago</t>
+  </si>
+  <si>
+    <t>Tarjeta de débito</t>
+  </si>
+  <si>
+    <t>Tarjeta de Crédito</t>
+  </si>
+  <si>
+    <t>Pago total: 100% del pago al momento de firmar contrato (Se aplica 5% de descuento al total del proyecto. De $53,103.26 USD a $50,448.10 USD).</t>
   </si>
 </sst>
 </file>
@@ -115,14 +245,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -209,7 +346,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,8 +375,32 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -286,86 +447,190 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="9" fontId="11" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="11" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="8" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
+    <cellStyle name="20% - Énfasis1" xfId="6" builtinId="30"/>
+    <cellStyle name="40% - Énfasis6" xfId="7" builtinId="51"/>
     <cellStyle name="Bueno" xfId="3" builtinId="26"/>
     <cellStyle name="Celda de comprobación" xfId="4" builtinId="23"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -373,7 +638,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="5" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
       <font>
         <b val="0"/>
@@ -390,7 +655,26 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -412,6 +696,7 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -511,19 +796,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{260CAE73-387D-4728-94B4-6CA7A8B0F168}" name="Tabla1" displayName="Tabla1" ref="A2:H14" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A2:H14" xr:uid="{260CAE73-387D-4728-94B4-6CA7A8B0F168}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F6F1872D-62D6-465A-9EB6-D1E64C7FD1EA}" name="N ITEM" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{05A4D583-BEEA-420F-8DC9-DB385506B921}" name="DESCRIPCIÓN" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{16119888-3FB2-48ED-BB90-CB4798528804}" name="NO. DE PARTE" dataDxfId="4" dataCellStyle="Moneda"/>
-    <tableColumn id="4" xr3:uid="{17DCB875-5E51-4C91-B16E-78560646B0A5}" name="PRECIO UNITARIO" dataDxfId="3" dataCellStyle="Moneda"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{260CAE73-387D-4728-94B4-6CA7A8B0F168}" name="Tabla1" displayName="Tabla1" ref="A2:I20" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A2:I20" xr:uid="{260CAE73-387D-4728-94B4-6CA7A8B0F168}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{F6F1872D-62D6-465A-9EB6-D1E64C7FD1EA}" name="N ITEM" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{05A4D583-BEEA-420F-8DC9-DB385506B921}" name="DESCRIPCIÓN" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{16119888-3FB2-48ED-BB90-CB4798528804}" name="NO. DE PARTE" dataDxfId="5" dataCellStyle="Moneda"/>
+    <tableColumn id="4" xr3:uid="{17DCB875-5E51-4C91-B16E-78560646B0A5}" name="PRECIO UNITARIO" dataDxfId="4" dataCellStyle="Moneda"/>
     <tableColumn id="8" xr3:uid="{9504F072-2CE8-4154-ADE6-5071E962149C}" name="DESCUENTOS"/>
-    <tableColumn id="5" xr3:uid="{DAECB143-E7A2-4C29-91CB-3EBCE0FFA4CA}" name="SUBTOTAL" dataDxfId="2" dataCellStyle="Moneda"/>
-    <tableColumn id="10" xr3:uid="{B913AF07-4667-4467-8BAC-58B0321E83ED}" name="TOTAL" dataDxfId="0" dataCellStyle="Moneda">
+    <tableColumn id="5" xr3:uid="{DAECB143-E7A2-4C29-91CB-3EBCE0FFA4CA}" name="SUBTOTAL" dataDxfId="3" dataCellStyle="Moneda"/>
+    <tableColumn id="10" xr3:uid="{B913AF07-4667-4467-8BAC-58B0321E83ED}" name="TOTAL" dataDxfId="1" dataCellStyle="Moneda">
       <calculatedColumnFormula>(C3*D3)*(100/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{CDC3B595-CE04-4E68-9C64-2BFC0D49CE76}" name="LINK" dataDxfId="1" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="9" xr3:uid="{1ADA9541-18CA-4B01-BDAC-D6008F0FAA29}" name="Dolares" dataDxfId="0" dataCellStyle="Moneda">
+      <calculatedColumnFormula>G3/$F23</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{CDC3B595-CE04-4E68-9C64-2BFC0D49CE76}" name="LINK" dataDxfId="2" dataCellStyle="Hipervínculo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -730,37 +1018,39 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="46.2" x14ac:dyDescent="0.85">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -773,20 +1063,23 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="16" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -796,25 +1089,29 @@
       <c r="C3" s="7">
         <v>15</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="13">
         <v>8969</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="17">
         <v>15</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="11">
         <f>C3*D3</f>
         <v>134535</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="12">
         <f t="shared" ref="G3:G11" si="0">(C3*D3)*(100/100)</f>
         <v>134535</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="12">
+        <f>G3/F23</f>
+        <v>7705.3264604810993</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -824,25 +1121,29 @@
       <c r="C4" s="7">
         <v>5</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="13">
         <v>11310</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="17">
         <v>5</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="11">
         <f>C4*D4</f>
         <v>56550</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="12">
         <f t="shared" si="0"/>
         <v>56550</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="12">
+        <f>G4/F23</f>
+        <v>3238.8316151202748</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -852,23 +1153,27 @@
       <c r="C5" s="7">
         <v>3</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="11">
         <v>30000</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="17">
         <v>0</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="11">
         <f>C5*D5</f>
         <v>90000</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="12">
         <f t="shared" si="0"/>
         <v>90000</v>
       </c>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="H5" s="12">
+        <f>G5/F23</f>
+        <v>5154.6391752577319</v>
+      </c>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -878,25 +1183,29 @@
       <c r="C6" s="7">
         <v>9</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="11">
         <v>1149</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="17">
         <v>10</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="11">
         <f>C6*D6</f>
         <v>10341</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="12">
         <f t="shared" si="0"/>
         <v>10341</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="12">
+        <f>G6/F23</f>
+        <v>592.26804123711338</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -906,25 +1215,29 @@
       <c r="C7" s="7">
         <v>5</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="11">
         <v>152.28</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="17">
         <v>0</v>
       </c>
-      <c r="F7" s="14">
-        <f t="shared" ref="F7:F12" si="1">C7*D7</f>
+      <c r="F7" s="11">
+        <f t="shared" ref="F7:F20" si="1">C7*D7</f>
         <v>761.4</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="12">
         <f t="shared" si="0"/>
         <v>761.4</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="12">
+        <f>G7/F23</f>
+        <v>43.608247422680407</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -934,23 +1247,27 @@
       <c r="C8" s="7">
         <v>120</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="11">
         <v>500</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="17">
         <v>0</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="11">
         <f t="shared" si="1"/>
         <v>60000</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="12">
         <f t="shared" si="0"/>
         <v>60000</v>
       </c>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="H8" s="12">
+        <f>G8/F23</f>
+        <v>3436.4261168384878</v>
+      </c>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -960,198 +1277,844 @@
       <c r="C9" s="7">
         <v>15</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="11">
         <v>2034.933</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="18">
         <v>0</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="11">
         <f t="shared" si="1"/>
         <v>30523.994999999999</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="12">
         <f t="shared" si="0"/>
         <v>30523.994999999999</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="12">
+        <f>G9/F23</f>
+        <v>1748.2242268041236</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="14">
         <v>15</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>1939.4</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="18">
         <v>0</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="11">
         <f t="shared" si="1"/>
         <v>29091</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="12">
         <f t="shared" si="0"/>
         <v>29091</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="12">
+        <f>G10/F23</f>
+        <v>1666.1512027491408</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="14">
         <v>15</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>1945.93</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="18">
         <v>0</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="11">
         <f t="shared" si="1"/>
         <v>29188.95</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="12">
         <f t="shared" si="0"/>
         <v>29188.95</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="12">
+        <f>G11/F23</f>
+        <v>1671.7611683848797</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="14">
         <v>15</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>2141.3330000000001</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="18">
         <v>0</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="11">
         <f t="shared" si="1"/>
         <v>32119.995000000003</v>
       </c>
-      <c r="G12" s="18">
-        <f t="shared" ref="G10:G12" si="2">(C12*D12)*(100/100)</f>
+      <c r="G12" s="12">
+        <f t="shared" ref="G12" si="2">(C12*D12)*(100/100)</f>
         <v>32119.995000000003</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="12">
+        <f>G12/F23</f>
+        <v>1839.6331615120275</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="14">
+        <v>4</v>
+      </c>
+      <c r="D13" s="12">
+        <v>21834.65</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
+        <f t="shared" si="1"/>
+        <v>87338.6</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" ref="G13:G18" si="3">(C13*D13)*(100/100)</f>
+        <v>87338.6</v>
+      </c>
+      <c r="H13" s="12">
+        <f>G13/F23</f>
+        <v>5002.2107674684994</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="17">
-        <v>4</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="22">
-        <f t="shared" ref="G13:G14" si="3">(C13*D13)*(100/100)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="22">
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="12">
+        <f>1312.51*2</f>
+        <v>2625.02</v>
+      </c>
+      <c r="E14" s="18">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
+        <f t="shared" si="1"/>
+        <v>2625.02</v>
+      </c>
+      <c r="G14" s="11">
+        <f>(C14*D14)*(100/100)</f>
+        <v>2625.02</v>
+      </c>
+      <c r="H14" s="12">
+        <f>G14/F23</f>
+        <v>150.34478808705612</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11">
+        <f>2*826.18</f>
+        <v>1652.36</v>
+      </c>
+      <c r="E15" s="18">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" si="1"/>
+        <v>1652.36</v>
+      </c>
+      <c r="G15" s="11">
+        <f>(C15*D15)*(100/100)</f>
+        <v>1652.36</v>
+      </c>
+      <c r="H15" s="12">
+        <f>G15/F23</f>
+        <v>94.636884306987383</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12">
+        <f>294.35 * 2</f>
+        <v>588.70000000000005</v>
+      </c>
+      <c r="E16" s="18">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11">
+        <f t="shared" si="1"/>
+        <v>588.70000000000005</v>
+      </c>
+      <c r="G16" s="11">
+        <f>(C16*D16)*(100/100)</f>
+        <v>588.70000000000005</v>
+      </c>
+      <c r="H16" s="12">
+        <f>G16/F23</f>
+        <v>33.717067583046962</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="12">
+        <f>464.99*2</f>
+        <v>929.98</v>
+      </c>
+      <c r="E17" s="18">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="1"/>
+        <v>929.98</v>
+      </c>
+      <c r="G17" s="11">
+        <f>(C17*D17)*(100/100)</f>
+        <v>929.98</v>
+      </c>
+      <c r="H17" s="12">
+        <f>G17/F23</f>
+        <v>53.263459335624283</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="14">
+        <v>4</v>
+      </c>
+      <c r="D18" s="12">
+        <v>15000</v>
+      </c>
+      <c r="E18" s="18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="G18" s="12">
         <f t="shared" si="3"/>
+        <v>60000</v>
+      </c>
+      <c r="H18" s="12">
+        <f>G18/F23</f>
+        <v>3436.4261168384878</v>
+      </c>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="14">
+        <v>4</v>
+      </c>
+      <c r="D19" s="12">
+        <v>30000</v>
+      </c>
+      <c r="E19" s="18">
         <v>0</v>
       </c>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="11">
-        <f>SUM(G3:G14)</f>
-        <v>473111.34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="21" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H34" s="2"/>
+      <c r="F19" s="11">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
+      <c r="G19" s="12">
+        <f>(C19*D19)*(100/100)</f>
+        <v>120000</v>
+      </c>
+      <c r="H19" s="12">
+        <f>G19/F23</f>
+        <v>6872.8522336769756</v>
+      </c>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="14">
+        <v>2</v>
+      </c>
+      <c r="D20" s="12">
+        <v>30000</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="11">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="G20" s="12">
+        <f>(C20*D20)*(100/100)</f>
+        <v>60000</v>
+      </c>
+      <c r="H20" s="12">
+        <f>G20/F23</f>
+        <v>3436.4261168384878</v>
+      </c>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="37">
+        <v>45061</v>
+      </c>
+      <c r="F22" s="37"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="26"/>
+      <c r="B23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="25">
+        <v>17.46</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="H23" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="28">
+        <f>SUM(Tabla1[TOTAL])</f>
+        <v>806246</v>
+      </c>
+      <c r="C24" s="30">
+        <f>SUM(Tabla1[Dolares])</f>
+        <v>46176.74684994272</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="33"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:10" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="22">
+        <v>0.15</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+    </row>
+    <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="22">
+        <v>2.25</v>
+      </c>
+      <c r="E28" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="35"/>
+      <c r="C30" s="36"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+    </row>
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="24">
+        <f>SUM(G3:G20)*1.15</f>
+        <v>927182.89999999991</v>
+      </c>
+      <c r="C32" s="24">
+        <f>B32/F23</f>
+        <v>53103.258877434127</v>
+      </c>
+      <c r="D32" s="23"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="24">
+        <f>B32*2*1.25</f>
+        <v>2317957.25</v>
+      </c>
+      <c r="C33" s="24">
+        <f>B33/F23</f>
+        <v>132758.14719358532</v>
+      </c>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="24">
+        <f>B33-B32</f>
+        <v>1390774.35</v>
+      </c>
+      <c r="C34" s="24">
+        <f>B34/F23</f>
+        <v>79654.888316151206</v>
+      </c>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="24">
+        <f>B34/30</f>
+        <v>46359.145000000004</v>
+      </c>
+      <c r="C35" s="24">
+        <f>B35/F23</f>
+        <v>2655.1629438717068</v>
+      </c>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="24">
+        <f>B35*0.3</f>
+        <v>13907.7435</v>
+      </c>
+      <c r="C36" s="24">
+        <f>B36/F23</f>
+        <v>796.54888316151198</v>
+      </c>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+    </row>
+    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="24">
+        <f>B35-B36</f>
+        <v>32451.401500000004</v>
+      </c>
+      <c r="C37" s="24">
+        <f>B37/F23</f>
+        <v>1858.6140607101947</v>
+      </c>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+    </row>
+    <row r="38" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+    </row>
+    <row r="39" spans="1:10" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="36"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+    </row>
+    <row r="40" spans="1:10" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="31">
+        <f>B45*0.25</f>
+        <v>33189.53679839633</v>
+      </c>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="31">
+        <f>B45*0.3</f>
+        <v>39827.444158075596</v>
+      </c>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="31">
+        <f>B45*0.4</f>
+        <v>53103.258877434127</v>
+      </c>
+      <c r="E42" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="38"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="31">
+        <f>B45*0.025</f>
+        <v>3318.953679839633</v>
+      </c>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="31">
+        <f>B45*0.025</f>
+        <v>3318.953679839633</v>
+      </c>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="31">
+        <f>C33</f>
+        <v>132758.14719358532</v>
+      </c>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="38"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="41"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F48" s="2"/>
+    </row>
+    <row r="52" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="39"/>
+      <c r="J52" s="39"/>
+    </row>
+    <row r="53" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="39"/>
+      <c r="J53" s="39"/>
+    </row>
+    <row r="54" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="39"/>
+    </row>
+    <row r="55" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="39"/>
+    </row>
+    <row r="56" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="39"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+  <mergeCells count="9">
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="E42:J45"/>
+    <mergeCell ref="E28:J41"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A30:C30"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{2421FD61-C521-45B2-8DF5-B7B485BF9E38}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{D9DB3FEB-3A05-490A-A601-E4659876CB25}"/>
-    <hyperlink ref="H6" r:id="rId3" xr:uid="{D18119C8-5FA6-4F43-8CD8-2A77CC41275D}"/>
-    <hyperlink ref="H10" r:id="rId4" xr:uid="{9BE40A90-D202-4C44-8466-BCB4BDBFE904}"/>
-    <hyperlink ref="H12" r:id="rId5" xr:uid="{A7BF6B39-7EEC-4D0C-A1BF-9776AEF5C3D7}"/>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{2421FD61-C521-45B2-8DF5-B7B485BF9E38}"/>
+    <hyperlink ref="I4" r:id="rId2" xr:uid="{D9DB3FEB-3A05-490A-A601-E4659876CB25}"/>
+    <hyperlink ref="I6" r:id="rId3" xr:uid="{D18119C8-5FA6-4F43-8CD8-2A77CC41275D}"/>
+    <hyperlink ref="I10" r:id="rId4" xr:uid="{9BE40A90-D202-4C44-8466-BCB4BDBFE904}"/>
+    <hyperlink ref="I12" r:id="rId5" xr:uid="{A7BF6B39-7EEC-4D0C-A1BF-9776AEF5C3D7}"/>
+    <hyperlink ref="I9" r:id="rId6" xr:uid="{9B74B351-3DA7-4DEA-A4D6-66E406BFB56F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+  <ignoredErrors>
+    <ignoredError sqref="H3:H5" calculatedColumn="1"/>
+  </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Prupuesta Económica V5.xlsx
</commit_message>
<xml_diff>
--- a/Ventas/Propuesta Económica/Prupuesta Económica V5.xlsx
+++ b/Ventas/Propuesta Económica/Prupuesta Económica V5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\AntirShadow\Documents\GitHub\ProyectoRedes\Ventas\Propuesta Económica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AntirShadow\Documents\GitHub\ProyectoRedes\Ventas\Propuesta Económica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853E359E-9EEB-4EB0-B920-FAF64FBDFBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22E69DD-6406-4F1D-B8B8-E7723ADE2EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2340" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>PROPUESTA ECONÓMICA</t>
   </si>
@@ -81,9 +81,6 @@
     <t>https://articulo.mercadolibre.com.mx/MLM-885299270-cable-de-red-utp-cat-6e-bobina-305m-exterior-_JM?matt_tool=28238160&amp;utm_source=google_shopping&amp;utm_medium=organic</t>
   </si>
   <si>
-    <t>Conector RJ45 Cat7 (100 piezas)</t>
-  </si>
-  <si>
     <t>https://articulo.mercadolibre.com.mx/MLM-1300594446-100-piezas-cable-cat6-rj45-conectores-cat6-cat5e-rj45utp-_JM#position=5&amp;search_layout=grid&amp;type=item&amp;tracking_id=d26aa09f-a4f7-44a7-b455-ec3998c093b6</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Total USD</t>
   </si>
   <si>
     <t>Pago inicial: 25%</t>
@@ -236,6 +230,15 @@
   </si>
   <si>
     <t>Pago total: 100% del pago al momento de firmar contrato (Se aplica 5% de descuento al total del proyecto. De $133,563.50 USD a $126,885.33 USD).</t>
+  </si>
+  <si>
+    <t>Impuestos Retenidos Por Persona</t>
+  </si>
+  <si>
+    <t>Cheques</t>
+  </si>
+  <si>
+    <t>Conector RJ45 Cat6 (100 piezas)</t>
   </si>
 </sst>
 </file>
@@ -243,10 +246,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -359,6 +362,15 @@
       <u val="singleAccounting"/>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -528,14 +540,14 @@
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -565,16 +577,16 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -588,8 +600,8 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
     <xf numFmtId="9" fontId="12" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="12" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -606,76 +618,79 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="9" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="4" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="8" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="6" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="8" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="4" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -708,7 +723,7 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -727,7 +742,7 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -746,7 +761,7 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -765,7 +780,7 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1071,37 +1086,41 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B12"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.5703125" customWidth="1"/>
+    <col min="1" max="1" width="47.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:9" ht="46.2" x14ac:dyDescent="0.85">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-    </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+    </row>
+    <row r="2" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1115,7 +1134,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -1124,13 +1143,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1140,21 +1159,21 @@
       <c r="C3" s="7">
         <v>15</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="33">
         <v>8969</v>
       </c>
       <c r="E3" s="16">
         <v>15</v>
       </c>
-      <c r="F3" s="47">
-        <f>C3*D3</f>
+      <c r="F3" s="34">
+        <f t="shared" ref="F3:F19" si="0">C3*D3</f>
         <v>134535</v>
       </c>
-      <c r="G3" s="48">
-        <f>(C3*D3)*(100/100)</f>
+      <c r="G3" s="14">
+        <f t="shared" ref="G3:G19" si="1">(C3*D3)*(100/100)</f>
         <v>134535</v>
       </c>
-      <c r="H3" s="48">
+      <c r="H3" s="14">
         <f>G3/Hoja1!F2</f>
         <v>7705.3264604810993</v>
       </c>
@@ -1162,7 +1181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1172,21 +1191,21 @@
       <c r="C4" s="7">
         <v>5</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="33">
         <v>11310</v>
       </c>
       <c r="E4" s="16">
         <v>5</v>
       </c>
-      <c r="F4" s="47">
-        <f>C4*D4</f>
+      <c r="F4" s="34">
+        <f t="shared" si="0"/>
         <v>56550</v>
       </c>
-      <c r="G4" s="48">
-        <f>(C4*D4)*(100/100)</f>
+      <c r="G4" s="14">
+        <f t="shared" si="1"/>
         <v>56550</v>
       </c>
-      <c r="H4" s="48">
+      <c r="H4" s="14">
         <f>G4/Hoja1!F2</f>
         <v>3238.8316151202748</v>
       </c>
@@ -1194,7 +1213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1204,51 +1223,51 @@
       <c r="C5" s="7">
         <v>3</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="34">
         <v>30000</v>
       </c>
       <c r="E5" s="16">
         <v>0</v>
       </c>
-      <c r="F5" s="47">
-        <f>C5*D5</f>
+      <c r="F5" s="34">
+        <f t="shared" si="0"/>
         <v>90000</v>
       </c>
-      <c r="G5" s="48">
-        <f>(C5*D5)*(100/100)</f>
+      <c r="G5" s="14">
+        <f t="shared" si="1"/>
         <v>90000</v>
       </c>
-      <c r="H5" s="48">
+      <c r="H5" s="14">
         <f>G5/Hoja1!F2</f>
         <v>5154.6391752577319</v>
       </c>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="55" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7">
         <v>9</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="34">
         <v>1149</v>
       </c>
       <c r="E6" s="16">
         <v>10</v>
       </c>
-      <c r="F6" s="47">
-        <f>C6*D6</f>
+      <c r="F6" s="34">
+        <f t="shared" si="0"/>
         <v>10341</v>
       </c>
-      <c r="G6" s="48">
-        <f>(C6*D6)*(100/100)</f>
+      <c r="G6" s="14">
+        <f t="shared" si="1"/>
         <v>10341</v>
       </c>
-      <c r="H6" s="48">
+      <c r="H6" s="14">
         <f>G6/Hoja1!F2</f>
         <v>592.26804123711338</v>
       </c>
@@ -1256,421 +1275,421 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>15</v>
+      <c r="B7" s="55" t="s">
+        <v>66</v>
       </c>
       <c r="C7" s="7">
         <v>5</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="34">
         <v>152.28</v>
       </c>
       <c r="E7" s="16">
         <v>0</v>
       </c>
-      <c r="F7" s="47">
-        <f>C7*D7</f>
+      <c r="F7" s="34">
+        <f t="shared" si="0"/>
         <v>761.4</v>
       </c>
-      <c r="G7" s="48">
-        <f>(C7*D7)*(100/100)</f>
+      <c r="G7" s="14">
+        <f t="shared" si="1"/>
         <v>761.4</v>
       </c>
-      <c r="H7" s="48">
+      <c r="H7" s="14">
         <f>G7/Hoja1!F2</f>
         <v>43.608247422680407</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="7">
         <v>120</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="34">
         <v>500</v>
       </c>
       <c r="E8" s="16">
         <v>0</v>
       </c>
-      <c r="F8" s="47">
-        <f>C8*D8</f>
+      <c r="F8" s="34">
+        <f t="shared" si="0"/>
         <v>60000</v>
       </c>
-      <c r="G8" s="48">
-        <f>(C8*D8)*(100/100)</f>
+      <c r="G8" s="14">
+        <f t="shared" si="1"/>
         <v>60000</v>
       </c>
-      <c r="H8" s="48">
+      <c r="H8" s="14">
         <f>G8/Hoja1!F2</f>
         <v>3436.4261168384878</v>
       </c>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="7">
         <v>15</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="34">
         <v>2034.933</v>
       </c>
       <c r="E9" s="17">
         <v>0</v>
       </c>
-      <c r="F9" s="47">
-        <f>C9*D9</f>
+      <c r="F9" s="34">
+        <f t="shared" si="0"/>
         <v>30523.994999999999</v>
       </c>
-      <c r="G9" s="48">
-        <f>(C9*D9)*(100/100)</f>
+      <c r="G9" s="14">
+        <f t="shared" si="1"/>
         <v>30523.994999999999</v>
       </c>
-      <c r="H9" s="48">
+      <c r="H9" s="14">
         <f>G9/Hoja1!F2</f>
         <v>1748.2242268041236</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="13">
         <v>15</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="14">
         <v>1939.4</v>
       </c>
       <c r="E10" s="17">
         <v>0</v>
       </c>
-      <c r="F10" s="47">
-        <f>C10*D10</f>
+      <c r="F10" s="34">
+        <f t="shared" si="0"/>
         <v>29091</v>
       </c>
-      <c r="G10" s="48">
-        <f>(C10*D10)*(100/100)</f>
+      <c r="G10" s="14">
+        <f t="shared" si="1"/>
         <v>29091</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10" s="14">
         <f>G10/Hoja1!F2</f>
         <v>1666.1512027491408</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="13">
         <v>15</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="14">
         <v>1945.93</v>
       </c>
       <c r="E11" s="17">
         <v>0</v>
       </c>
-      <c r="F11" s="47">
-        <f>C11*D11</f>
+      <c r="F11" s="34">
+        <f t="shared" si="0"/>
         <v>29188.95</v>
       </c>
-      <c r="G11" s="48">
-        <f>(C11*D11)*(100/100)</f>
+      <c r="G11" s="14">
+        <f t="shared" si="1"/>
         <v>29188.95</v>
       </c>
-      <c r="H11" s="48">
+      <c r="H11" s="14">
         <f>G11/Hoja1!F2</f>
         <v>1671.7611683848797</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="13">
         <v>15</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="14">
         <v>2141.3330000000001</v>
       </c>
       <c r="E12" s="17">
         <v>0</v>
       </c>
-      <c r="F12" s="47">
-        <f>C12*D12</f>
+      <c r="F12" s="34">
+        <f t="shared" si="0"/>
         <v>32119.995000000003</v>
       </c>
-      <c r="G12" s="48">
-        <f>(C12*D12)*(100/100)</f>
+      <c r="G12" s="14">
+        <f t="shared" si="1"/>
         <v>32119.995000000003</v>
       </c>
-      <c r="H12" s="48">
+      <c r="H12" s="14">
         <f>G12/Hoja1!F2</f>
         <v>1839.6331615120275</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="13">
         <v>4</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="14">
         <v>21834.65</v>
       </c>
       <c r="E13" s="17">
         <v>0</v>
       </c>
-      <c r="F13" s="47">
-        <f>C13*D13</f>
+      <c r="F13" s="34">
+        <f t="shared" si="0"/>
         <v>87338.6</v>
       </c>
-      <c r="G13" s="48">
-        <f>(C13*D13)*(100/100)</f>
+      <c r="G13" s="14">
+        <f t="shared" si="1"/>
         <v>87338.6</v>
       </c>
-      <c r="H13" s="48">
+      <c r="H13" s="14">
         <f>G13/Hoja1!F2</f>
         <v>5002.2107674684994</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="7">
         <v>1</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="14">
         <f>1312.51*2</f>
         <v>2625.02</v>
       </c>
       <c r="E14" s="17">
         <v>0</v>
       </c>
-      <c r="F14" s="47">
-        <f>C14*D14</f>
+      <c r="F14" s="34">
+        <f t="shared" si="0"/>
         <v>2625.02</v>
       </c>
-      <c r="G14" s="47">
-        <f>(C14*D14)*(100/100)</f>
+      <c r="G14" s="34">
+        <f t="shared" si="1"/>
         <v>2625.02</v>
       </c>
-      <c r="H14" s="48">
+      <c r="H14" s="14">
         <f>G14/Hoja1!F2</f>
         <v>150.34478808705612</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="7">
         <v>1</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="34">
         <f>2*826.18</f>
         <v>1652.36</v>
       </c>
       <c r="E15" s="17">
         <v>0</v>
       </c>
-      <c r="F15" s="47">
-        <f>C15*D15</f>
+      <c r="F15" s="34">
+        <f t="shared" si="0"/>
         <v>1652.36</v>
       </c>
-      <c r="G15" s="47">
-        <f>(C15*D15)*(100/100)</f>
+      <c r="G15" s="34">
+        <f t="shared" si="1"/>
         <v>1652.36</v>
       </c>
-      <c r="H15" s="48">
+      <c r="H15" s="14">
         <f>G15/Hoja1!F2</f>
         <v>94.636884306987383</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="14">
         <f>294.35 * 2</f>
         <v>588.70000000000005</v>
       </c>
       <c r="E16" s="17">
         <v>0</v>
       </c>
-      <c r="F16" s="47">
-        <f>C16*D16</f>
+      <c r="F16" s="34">
+        <f t="shared" si="0"/>
         <v>588.70000000000005</v>
       </c>
-      <c r="G16" s="47">
-        <f>(C16*D16)*(100/100)</f>
+      <c r="G16" s="34">
+        <f t="shared" si="1"/>
         <v>588.70000000000005</v>
       </c>
-      <c r="H16" s="48">
+      <c r="H16" s="14">
         <f>G16/Hoja1!F2</f>
         <v>33.717067583046962</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="14">
         <f>464.99*2</f>
         <v>929.98</v>
       </c>
       <c r="E17" s="17">
         <v>0</v>
       </c>
-      <c r="F17" s="47">
-        <f>C17*D17</f>
+      <c r="F17" s="34">
+        <f t="shared" si="0"/>
         <v>929.98</v>
       </c>
-      <c r="G17" s="47">
-        <f>(C17*D17)*(100/100)</f>
+      <c r="G17" s="34">
+        <f t="shared" si="1"/>
         <v>929.98</v>
       </c>
-      <c r="H17" s="48">
+      <c r="H17" s="14">
         <f>G17/Hoja1!F2</f>
         <v>53.263459335624283</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="13">
         <v>4</v>
       </c>
-      <c r="D18" s="48">
+      <c r="D18" s="14">
         <v>15000</v>
       </c>
       <c r="E18" s="17">
         <v>0</v>
       </c>
-      <c r="F18" s="47">
-        <f>C18*D18</f>
+      <c r="F18" s="34">
+        <f t="shared" si="0"/>
         <v>60000</v>
       </c>
-      <c r="G18" s="48">
-        <f>(C18*D18)*(100/100)</f>
+      <c r="G18" s="14">
+        <f t="shared" si="1"/>
         <v>60000</v>
       </c>
-      <c r="H18" s="48">
+      <c r="H18" s="14">
         <f>G18/Hoja1!F2</f>
         <v>3436.4261168384878</v>
       </c>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="13">
         <v>4</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="14">
         <v>30000</v>
       </c>
       <c r="E19" s="17">
         <v>0</v>
       </c>
-      <c r="F19" s="47">
-        <f>C19*D19</f>
+      <c r="F19" s="34">
+        <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-      <c r="G19" s="48">
-        <f>(C19*D19)*(100/100)</f>
+      <c r="G19" s="14">
+        <f t="shared" si="1"/>
         <v>120000</v>
       </c>
-      <c r="H19" s="48">
+      <c r="H19" s="14">
         <f>G19/Hoja1!F2</f>
         <v>6872.8522336769756</v>
       </c>
       <c r="I19" s="8"/>
     </row>
-    <row r="20" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="6"/>
       <c r="C20" s="13"/>
@@ -1681,22 +1700,22 @@
       <c r="H20" s="12"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:9" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:9" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="6:6" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="6:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="6:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="6:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="6:6" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="6:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="6:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="6:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F47" s="2"/>
     </row>
-    <row r="51" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E51" s="26"/>
       <c r="F51" s="26"/>
       <c r="G51" s="26"/>
@@ -1704,7 +1723,7 @@
       <c r="I51" s="26"/>
       <c r="J51" s="26"/>
     </row>
-    <row r="52" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E52" s="26"/>
       <c r="F52" s="26"/>
       <c r="G52" s="26"/>
@@ -1712,7 +1731,7 @@
       <c r="I52" s="26"/>
       <c r="J52" s="26"/>
     </row>
-    <row r="53" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E53" s="26"/>
       <c r="F53" s="26"/>
       <c r="G53" s="26"/>
@@ -1720,7 +1739,7 @@
       <c r="I53" s="26"/>
       <c r="J53" s="26"/>
     </row>
-    <row r="54" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E54" s="26"/>
       <c r="F54" s="26"/>
       <c r="G54" s="26"/>
@@ -1728,7 +1747,7 @@
       <c r="I54" s="26"/>
       <c r="J54" s="26"/>
     </row>
-    <row r="55" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E55" s="26"/>
       <c r="F55" s="26"/>
       <c r="G55" s="26"/>
@@ -1747,14 +1766,15 @@
     <hyperlink ref="I10" r:id="rId4" xr:uid="{9BE40A90-D202-4C44-8466-BCB4BDBFE904}"/>
     <hyperlink ref="I12" r:id="rId5" xr:uid="{A7BF6B39-7EEC-4D0C-A1BF-9776AEF5C3D7}"/>
     <hyperlink ref="I9" r:id="rId6" xr:uid="{9B74B351-3DA7-4DEA-A4D6-66E406BFB56F}"/>
+    <hyperlink ref="I7" r:id="rId7" location="position=5&amp;search_layout=grid&amp;type=item&amp;tracking_id=d26aa09f-a4f7-44a7-b455-ec3998c093b6" xr:uid="{4865831C-F97A-455F-9B3E-7D7A9C269B34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
   <ignoredErrors>
     <ignoredError sqref="H3:H5" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1764,188 +1784,191 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="E7" sqref="E7:J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="47.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+    <row r="1" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
       <c r="D1" s="12"/>
-      <c r="E1" s="38">
+      <c r="E1" s="48">
         <v>45061</v>
       </c>
-      <c r="F1" s="38"/>
+      <c r="F1" s="48"/>
       <c r="G1" s="12"/>
       <c r="H1" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23"/>
       <c r="B2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="45">
+        <v>41</v>
+      </c>
+      <c r="F2" s="32">
         <v>17.46</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="43">
+        <v>46</v>
+      </c>
+      <c r="B3" s="30">
         <f>SUM(Tabla1[TOTAL])</f>
         <v>746246</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="31">
         <f>SUM(Tabla1[Dolares])</f>
         <v>42740.320733104229</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="22" t="s">
         <v>44</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>45</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="13"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="40"/>
+      <c r="H4" s="39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="50"/>
       <c r="C5" s="13"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="19">
         <v>0.15</v>
       </c>
-      <c r="E6" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E6" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+    </row>
+    <row r="7" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="19">
         <v>2.25</v>
       </c>
-      <c r="E7" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-    </row>
-    <row r="8" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-    </row>
-    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="31"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
+      <c r="E7" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+    </row>
+    <row r="8" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="52"/>
+      <c r="C9" s="53"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="36"/>
       <c r="B10" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" spans="1:10" ht="17.25" thickTop="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+    </row>
+    <row r="11" spans="1:10" ht="16.2" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A11" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="21">
         <f>B3*1.25</f>
         <v>932807.5</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="35">
         <f>B11/F2</f>
         <v>53425.400916380298</v>
       </c>
       <c r="D11" s="20"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+    </row>
+    <row r="12" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="21">
         <f>B11*2*1.25</f>
@@ -1955,16 +1978,16 @@
         <f>B12/F2</f>
         <v>133563.50229095074</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+    </row>
+    <row r="13" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="21">
         <f>B12-B11</f>
@@ -1974,16 +1997,16 @@
         <f>B13/F2</f>
         <v>80138.10137457044</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+    </row>
+    <row r="14" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="21">
         <f>B13/30</f>
@@ -1993,16 +2016,16 @@
         <f>B14/F2</f>
         <v>2671.2700458190147</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-    </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+    </row>
+    <row r="15" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B15" s="21">
         <f>B14*0.3</f>
@@ -2012,16 +2035,16 @@
         <f>B15/F2</f>
         <v>801.38101374570442</v>
       </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-    </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+    </row>
+    <row r="16" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="21">
         <f>B14-B15</f>
@@ -2031,52 +2054,52 @@
         <f>B16/F2</f>
         <v>1869.8890320733103</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-    </row>
-    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+    </row>
+    <row r="18" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+    </row>
+    <row r="19" spans="1:10" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+    </row>
+    <row r="20" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="21">
         <f>B25*0.25</f>
@@ -2086,16 +2109,16 @@
         <f>C25*0.25</f>
         <v>33390.875572737685</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-    </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+    </row>
+    <row r="21" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" s="21">
         <f>B25*0.3</f>
@@ -2105,18 +2128,18 @@
         <f>C25*0.3</f>
         <v>40069.05068728522</v>
       </c>
-      <c r="E21" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-    </row>
-    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E21" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+    </row>
+    <row r="22" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="21">
         <f>B25*0.4</f>
@@ -2126,16 +2149,16 @@
         <f>C25*0.4</f>
         <v>53425.400916380298</v>
       </c>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-    </row>
-    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+    </row>
+    <row r="23" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23" s="21">
         <f>B25*0.25</f>
@@ -2145,16 +2168,16 @@
         <f>C25*0.025</f>
         <v>3339.0875572737687</v>
       </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-    </row>
-    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+    </row>
+    <row r="24" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="21">
         <f>B25*0.25</f>
@@ -2165,16 +2188,16 @@
         <v>3339.0875572737687</v>
       </c>
       <c r="D24" s="20"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-    </row>
-    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+    </row>
+    <row r="25" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="21">
         <f>B12</f>
@@ -2191,7 +2214,7 @@
       <c r="I25" s="27"/>
       <c r="J25" s="27"/>
     </row>
-    <row r="26" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
@@ -2199,8 +2222,8 @@
       <c r="I26" s="27"/>
       <c r="J26" s="27"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G29" s="53"/>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G29" s="38"/>
       <c r="H29" s="20"/>
     </row>
   </sheetData>
@@ -2215,5 +2238,6 @@
     <mergeCell ref="A18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>